<commit_message>
Updates ftw. Should be ready for multiple motor configs now.
</commit_message>
<xml_diff>
--- a/resources/hardwareList.xlsx
+++ b/resources/hardwareList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="460" windowWidth="21600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Stages" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="92">
   <si>
     <t>Stage</t>
   </si>
@@ -222,9 +222,6 @@
     <t>Accuracy</t>
   </si>
   <si>
-    <t>Range</t>
-  </si>
-  <si>
     <t>Detector</t>
   </si>
   <si>
@@ -280,13 +277,40 @@
   </si>
   <si>
     <t>Dependency can inform the system (particularly for translations on top of rotations) if any re-calculation is required.</t>
+  </si>
+  <si>
+    <t>(mm) or (deg)</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>-motor</t>
+  </si>
+  <si>
+    <t>large tx(x)/tx/rx</t>
+  </si>
+  <si>
+    <t>Motor Label</t>
+  </si>
+  <si>
+    <t>EPICS PV</t>
+  </si>
+  <si>
+    <t>Application Order</t>
+  </si>
+  <si>
+    <t>Center of Rotation in (mm) above top plate</t>
+  </si>
+  <si>
+    <t>CoR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -300,6 +324,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -323,11 +354,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,92 +645,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="71" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="G1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
-        <v>78</v>
-      </c>
+    </row>
+    <row r="2" spans="1:9" s="6" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>1E-3</v>
       </c>
       <c r="I3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -698,16 +750,22 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>1E-3</v>
       </c>
       <c r="I4" t="s">
         <v>77</v>
@@ -718,13 +776,22 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1E-3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -732,7 +799,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>55</v>
@@ -746,19 +813,13 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -766,13 +827,25 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1E-3</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -780,13 +853,13 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -794,13 +867,13 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -808,13 +881,13 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -822,27 +895,27 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -850,14 +923,13 @@
         <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="1"/>
+        <v>60</v>
+      </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -865,13 +937,14 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C15" s="1"/>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -879,143 +952,163 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="H17">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="H18">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>28</v>
       </c>
       <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" t="s">
+      <c r="C20" s="1"/>
+      <c r="D20" t="s">
         <v>35</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>43</v>
       </c>
       <c r="D23" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>43</v>
       </c>
       <c r="D25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" t="s">
         <v>52</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E26" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="B30" t="s">
         <v>80</v>
       </c>
-      <c r="B29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B30" t="s">
-        <v>83</v>
+      <c r="B31" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1044,42 +1137,42 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
         <v>65</v>
-      </c>
-      <c r="B1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" t="s">
-        <v>66</v>
       </c>
       <c r="F1" t="s">
         <v>9</v>
       </c>
       <c r="G1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" t="s">
         <v>73</v>
-      </c>
-      <c r="H1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D2">
         <v>0.2</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G2">
         <v>1E-3</v>

</xml_diff>